<commit_message>
Vendor Synthetic Data Generated
</commit_message>
<xml_diff>
--- a/definitions/vendor.xlsx
+++ b/definitions/vendor.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="152">
   <si>
     <t>TABLE_NAME</t>
   </si>
@@ -61,58 +61,58 @@
     <t xml:space="preserve">80    </t>
   </si>
   <si>
+    <t>generate_lifnr_yn01()</t>
+  </si>
+  <si>
+    <t>A custom function that generates random Supplier IDs based on the company name.</t>
+  </si>
+  <si>
+    <t>BU_GROUP</t>
+  </si>
+  <si>
+    <t>default("YNO1")</t>
+  </si>
+  <si>
+    <t>According to Vendor Mapping: Use default 'YN01'</t>
+  </si>
+  <si>
+    <t>KTOKK</t>
+  </si>
+  <si>
+    <t>default("SUPL")</t>
+  </si>
+  <si>
+    <t>According to Vendor Mapping: Use default 'SUPL'</t>
+  </si>
+  <si>
+    <t>NAME_FIRST_P</t>
+  </si>
+  <si>
+    <t>optional_first_name()</t>
+  </si>
+  <si>
+    <t>A custom function that generates random first names. Based on a configurable probability, it may either generate a fake first name or leave it as null.</t>
+  </si>
+  <si>
+    <t>NAME_LAST_P</t>
+  </si>
+  <si>
+    <t>conditional_last_name(FIRST_NAME_P)</t>
+  </si>
+  <si>
+    <t>A custom function that generates random last names. It checks the first name: if it's null, the last name will also be null; otherwise, it generates a last name.</t>
+  </si>
+  <si>
+    <t>BPEXT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20    </t>
+  </si>
+  <si>
     <t>supplier_id_from_name(NAME_FIRST)</t>
   </si>
   <si>
-    <t>A custom function that generates random Supplier IDs based on the company name.</t>
-  </si>
-  <si>
-    <t>BU_GROUP</t>
-  </si>
-  <si>
-    <t>default("YNO1")</t>
-  </si>
-  <si>
-    <t>According to Vendor Mapping: Use default 'YN01'</t>
-  </si>
-  <si>
-    <t>KTOKK</t>
-  </si>
-  <si>
-    <t>default("SUPL")</t>
-  </si>
-  <si>
-    <t>According to Vendor Mapping: Use default 'SUPL'</t>
-  </si>
-  <si>
-    <t>NAME_FIRST_P</t>
-  </si>
-  <si>
-    <t>optional_first_name()</t>
-  </si>
-  <si>
-    <t>A custom function that generates random first names. Based on a configurable probability, it may either generate a fake first name or leave it as null.</t>
-  </si>
-  <si>
-    <t>NAME_LAST_P</t>
-  </si>
-  <si>
-    <t>conditional_last_name(FIRST_NAME_P)</t>
-  </si>
-  <si>
-    <t>A custom function that generates random last names. It checks the first name: if it's null, the last name will also be null; otherwise, it generates a last name.</t>
-  </si>
-  <si>
-    <t>BPEXT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20    </t>
-  </si>
-  <si>
-    <t>copy_value(LIFNR)</t>
-  </si>
-  <si>
-    <t>Same value as the LIFNR, based on the sample data.</t>
+    <t xml:space="preserve">Same value as the LIFNR, based on the sample data </t>
   </si>
   <si>
     <t>STREET</t>
@@ -261,6 +261,9 @@
     <t>AKONT</t>
   </si>
   <si>
+    <t>get_reconciliation_account("S_SUPPL_GEN", "LIFNR","COUNTRY",LIFNR)</t>
+  </si>
+  <si>
     <t>I'm not sure what the expected values look like, and the field descriptions aren't very clear. Could you share a few sample values?</t>
   </si>
   <si>
@@ -318,6 +321,9 @@
     <t xml:space="preserve">70    </t>
   </si>
   <si>
+    <t>lookup_parent_value("S_SUPPL_GEN", "LIFNR","CITY1",LIFNR)</t>
+  </si>
+  <si>
     <t>NOTE: The Supplier ID field in the sample data comes empty — should I leave it as null?</t>
   </si>
   <si>
@@ -361,6 +367,9 @@
   </si>
   <si>
     <t>PARVW</t>
+  </si>
+  <si>
+    <t>get_random_partner_function()</t>
   </si>
   <si>
     <t>NOTE: could we assign these values randomly — RS, WL, LF, BA?</t>
@@ -397,7 +406,7 @@
     <t xml:space="preserve">15    </t>
   </si>
   <si>
-    <t/>
+    <t>generate_bank_key(BANKS)</t>
   </si>
   <si>
     <t>BANKN</t>
@@ -430,25 +439,40 @@
     <t xml:space="preserve">2     </t>
   </si>
   <si>
+    <t>generate_bkont(BANKS)</t>
+  </si>
+  <si>
     <t>BKREF</t>
   </si>
   <si>
     <t>KOINH</t>
   </si>
   <si>
+    <t>lookup_parent_value("S_SUPPL_GEN", "LIFNR","NAME_FIRST",LIFNR)</t>
+  </si>
+  <si>
     <t>EBPP_ACCNAME</t>
   </si>
   <si>
+    <t>lookup_parent_value("S_SUPPL_GEN", "LIFNR","NAME_FIRST_P",LIFNR)</t>
+  </si>
+  <si>
     <t>S_SUPPL_TAXNUMBERS</t>
   </si>
   <si>
     <t>TAXTYPE</t>
   </si>
   <si>
+    <t>random_tax_type()</t>
+  </si>
+  <si>
     <t>Note: the sample data includes two categories — "X" and NULL. Should we use them?</t>
   </si>
   <si>
     <t>TAXNUM</t>
+  </si>
+  <si>
+    <t>generate_tax_number()</t>
   </si>
   <si>
     <t>Custom functions that generate random fake tax numbers.</t>
@@ -527,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -543,9 +567,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -864,15 +885,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="27.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="17.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="9.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="79.14785714285713" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="123.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="27.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="17.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="7.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="9.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="79.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="123.14785714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1192,7 +1213,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1" t="s">
         <v>59</v>
       </c>
@@ -1212,7 +1233,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1" t="s">
         <v>59</v>
       </c>
@@ -1232,7 +1253,7 @@
         <v>64</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1" t="s">
         <v>65</v>
       </c>
@@ -1252,7 +1273,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1" t="s">
         <v>66</v>
       </c>
@@ -1272,7 +1293,7 @@
         <v>67</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1" t="s">
         <v>66</v>
       </c>
@@ -1292,7 +1313,7 @@
         <v>70</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
       <c r="A22" s="1" t="s">
         <v>71</v>
       </c>
@@ -1312,7 +1333,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
       <c r="A23" s="1" t="s">
         <v>71</v>
       </c>
@@ -1332,7 +1353,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1" t="s">
         <v>75</v>
       </c>
@@ -1352,7 +1373,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="33">
       <c r="A25" s="1" t="s">
         <v>75</v>
       </c>
@@ -1372,7 +1393,7 @@
         <v>78</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1" t="s">
         <v>75</v>
       </c>
@@ -1385,17 +1406,19 @@
       <c r="D26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="F26" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25" hidden="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>8</v>
@@ -1405,15 +1428,15 @@
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25" hidden="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>8</v>
@@ -1423,12 +1446,12 @@
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25" hidden="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
       <c r="A29" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>12</v>
@@ -1443,12 +1466,12 @@
         <v>60</v>
       </c>
       <c r="F29" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+      <c r="A30" s="1" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25" hidden="1">
-      <c r="A30" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>76</v>
@@ -1466,9 +1489,9 @@
         <v>78</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
       <c r="A31" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>12</v>
@@ -1486,32 +1509,32 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
       <c r="A32" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
+      <c r="A33" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25" hidden="1">
-      <c r="A33" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="B33" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>8</v>
@@ -1520,18 +1543,18 @@
         <v>13</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25" hidden="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
       <c r="A34" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>8</v>
@@ -1541,15 +1564,15 @@
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25" hidden="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
       <c r="A35" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>8</v>
@@ -1558,36 +1581,38 @@
         <v>13</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25" hidden="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
       <c r="A36" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E36" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="F36" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25" hidden="1">
+        <v>101</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
       <c r="A37" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>8</v>
@@ -1596,44 +1621,44 @@
         <v>13</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25" hidden="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="F38" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25" hidden="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>69</v>
@@ -1642,18 +1667,18 @@
         <v>70</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>69</v>
@@ -1662,38 +1687,38 @@
         <v>70</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
       <c r="A41" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
+      <c r="A42" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25" hidden="1">
-      <c r="A42" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>69</v>
@@ -1702,9 +1727,9 @@
         <v>70</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
       <c r="A43" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>12</v>
@@ -1722,12 +1747,12 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
       <c r="A44" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>8</v>
@@ -1736,36 +1761,38 @@
         <v>13</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25" hidden="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
       <c r="A45" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
+      <c r="A46" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E45" s="2"/>
-      <c r="F45" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25" hidden="1">
-      <c r="A46" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="B46" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>8</v>
@@ -1773,23 +1800,25 @@
       <c r="D46" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E46" s="2"/>
+      <c r="E46" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="F46" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25" hidden="1">
+        <v>119</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
       <c r="A47" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>69</v>
@@ -1798,9 +1827,9 @@
         <v>70</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
       <c r="A48" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>12</v>
@@ -1818,9 +1847,9 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
       <c r="A49" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>12</v>
@@ -1838,12 +1867,12 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="33">
       <c r="A50" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>8</v>
@@ -1852,96 +1881,98 @@
         <v>13</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F50" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25">
+      <c r="A51" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25" hidden="1">
-      <c r="A51" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="B51" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>125</v>
+        <v>127</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="17.25" hidden="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="17.25">
       <c r="A52" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="17.25" hidden="1">
+        <v>132</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="17.25">
       <c r="A53" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="17.25" hidden="1">
+        <v>136</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="17.25">
       <c r="A54" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E54" s="2"/>
+        <v>138</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>139</v>
+      </c>
       <c r="F54" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="17.25" hidden="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="17.25">
       <c r="A55" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>8</v>
@@ -1949,17 +1980,19 @@
       <c r="D55" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E55" s="2"/>
+      <c r="E55" s="2" t="s">
+        <v>139</v>
+      </c>
       <c r="F55" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="17.25" hidden="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="17.25">
       <c r="A56" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>8</v>
@@ -1967,17 +2000,19 @@
       <c r="D56" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E56" s="2"/>
+      <c r="E56" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="F56" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="17.25" hidden="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="17.25">
       <c r="A57" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>8</v>
@@ -1985,17 +2020,19 @@
       <c r="D57" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E57" s="2"/>
+      <c r="E57" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="F57" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="17.25" hidden="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="17.25">
       <c r="A58" s="1" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>8</v>
@@ -2003,17 +2040,19 @@
       <c r="D58" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E58" s="2"/>
-      <c r="F58" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="17.25" hidden="1">
+      <c r="E58" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="17.25">
       <c r="A59" s="1" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>8</v>
@@ -2021,9 +2060,11 @@
       <c r="D59" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E59" s="2"/>
+      <c r="E59" s="2" t="s">
+        <v>150</v>
+      </c>
       <c r="F59" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>